<commit_message>
Teste funcional Gustavo e att relatorio legado
</commit_message>
<xml_diff>
--- a/Testes/Relatório_Legado.xlsx
+++ b/Testes/Relatório_Legado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuli\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\syloPrime\Testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864216EC-8933-4194-A9BA-8904D65F7A54}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731D83A9-2FAF-4400-9684-2B0698BBC3AB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5D089B20-8D19-4900-AD38-3F8CD4F45222}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
   <si>
     <t>FUNCIONALIDADE</t>
   </si>
@@ -97,6 +97,39 @@
   </si>
   <si>
     <t>Alerta não disparado, campos aceitando valores nulos ou &lt; 0</t>
+  </si>
+  <si>
+    <t>Cadastro</t>
+  </si>
+  <si>
+    <t>Cadastro sucesso</t>
+  </si>
+  <si>
+    <t>Cadastro sem cnpj</t>
+  </si>
+  <si>
+    <t>Cadastro sem E-mail</t>
+  </si>
+  <si>
+    <t>Cadastro sem senha</t>
+  </si>
+  <si>
+    <t>Cadastro efetuado com sucesso</t>
+  </si>
+  <si>
+    <t>Interação de telas</t>
+  </si>
+  <si>
+    <t>Site Institucional</t>
+  </si>
+  <si>
+    <t>Site Funcional</t>
+  </si>
+  <si>
+    <t>Parte Cadastro/Login</t>
+  </si>
+  <si>
+    <t>Interação funcionando normalmente</t>
   </si>
 </sst>
 </file>
@@ -198,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,6 +260,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -235,6 +271,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DA1D05-D473-42B0-9FEF-9FDDFCC050DE}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +623,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -601,7 +640,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
@@ -616,7 +655,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
@@ -631,7 +670,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -648,7 +687,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
@@ -663,7 +702,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -678,7 +717,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
@@ -692,54 +731,114 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3"/>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="3"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -861,9 +960,11 @@
       <c r="E32" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>